<commit_message>
Participant 3 baseline trend correction
analysis run just in case if needed for post defense edits
</commit_message>
<xml_diff>
--- a/data/Tau Dissertation Data.xlsx
+++ b/data/Tau Dissertation Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/dissertation_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409DB0A9-C3D0-F042-A41E-A15B5B8DC224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4D754A-F292-1148-A1C2-9C81F16F74E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37040" yWindow="4560" windowWidth="27240" windowHeight="15200" activeTab="1" xr2:uid="{F203A932-FAE8-884F-A6A8-A419375FF604}"/>
+    <workbookView xWindow="37040" yWindow="4560" windowWidth="27240" windowHeight="15200" activeTab="2" xr2:uid="{F203A932-FAE8-884F-A6A8-A419375FF604}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="1 and 2 corrected baseline" sheetId="2" r:id="rId2"/>
+    <sheet name="3 corrected baseline" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
   <si>
     <t>Participant 1</t>
   </si>
@@ -206,13 +207,61 @@
   </si>
   <si>
     <t>0.2007&lt;&gt;1</t>
+  </si>
+  <si>
+    <t>0.0033&lt;&gt;0.8123</t>
+  </si>
+  <si>
+    <t>0.0683&lt;&gt;0.7473</t>
+  </si>
+  <si>
+    <t>0.1106&lt;&gt;0.7050</t>
+  </si>
+  <si>
+    <t>#3+#4+#6</t>
+  </si>
+  <si>
+    <t>-0.812&lt;&gt;0.312</t>
+  </si>
+  <si>
+    <t>-0.742&lt;&gt;0.242</t>
+  </si>
+  <si>
+    <t>P3 BL vs P3 I</t>
+  </si>
+  <si>
+    <t>0.452&lt;&gt;1</t>
+  </si>
+  <si>
+    <t>0.520&lt;&gt;1</t>
+  </si>
+  <si>
+    <t>P2 BL vs P2 I</t>
+  </si>
+  <si>
+    <t>-0.182&lt;&gt;1</t>
+  </si>
+  <si>
+    <t>-0.101&lt;&gt;1</t>
+  </si>
+  <si>
+    <t>P1 BL vs P1 I</t>
+  </si>
+  <si>
+    <t>P3 BL vs P3 BL</t>
+  </si>
+  <si>
+    <t>P2 BL vs P2 BL</t>
+  </si>
+  <si>
+    <t>P1 BL vs P1 BL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -226,6 +275,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -272,10 +326,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -284,9 +339,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D033CA9D-BBF3-684C-9954-0BEBAF97EF57}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1056,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9325E4C0-27FB-334F-BC82-B59D29245E85}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
@@ -1884,4 +1941,466 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA828D8-E668-7540-9941-CBBA89FDF165}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="13" width="9.1640625" style="6" customWidth="1"/>
+    <col min="14" max="256" width="8.83203125" style="6" customWidth="1"/>
+    <col min="257" max="16384" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="G3" s="6">
+        <v>3.6667000000000001</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.9149</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.63829999999999998</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.5222</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.60150000000000003</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="6">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6">
+        <v>-6.6699999999999995E-2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>28.333300000000001</v>
+      </c>
+      <c r="H4" s="6">
+        <v>5.3228999999999997</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.35489999999999999</v>
+      </c>
+      <c r="J4" s="6">
+        <v>-0.18790000000000001</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="6">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.82140000000000002</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.83640000000000003</v>
+      </c>
+      <c r="G5" s="6">
+        <v>65.333299999999994</v>
+      </c>
+      <c r="H5" s="6">
+        <v>8.0829000000000004</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.28870000000000001</v>
+      </c>
+      <c r="J5" s="6">
+        <v>2.8454999999999999</v>
+      </c>
+      <c r="K5" s="6">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="6">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.82140000000000002</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.83640000000000003</v>
+      </c>
+      <c r="G6" s="6">
+        <v>65.333299999999994</v>
+      </c>
+      <c r="H6" s="6">
+        <v>8.0829000000000004</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.28870000000000001</v>
+      </c>
+      <c r="J6" s="6">
+        <v>2.8454999999999999</v>
+      </c>
+      <c r="K6" s="6">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="6">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.4667</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>140</v>
+      </c>
+      <c r="H8" s="6">
+        <v>11.8322</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.39439999999999997</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1.1832</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.23669999999999999</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="6">
+        <v>42</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <v>196</v>
+      </c>
+      <c r="H9" s="6">
+        <v>14</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="J9" s="6">
+        <v>3</v>
+      </c>
+      <c r="K9" s="6">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-10</v>
+      </c>
+      <c r="D11" s="6">
+        <v>40</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-0.25</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-0.25969999999999999</v>
+      </c>
+      <c r="G11" s="6">
+        <v>186.66669999999999</v>
+      </c>
+      <c r="H11" s="6">
+        <v>13.662599999999999</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.34160000000000001</v>
+      </c>
+      <c r="J11" s="6">
+        <v>-0.7319</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.4642</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.4078</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.2064</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.976</v>
+      </c>
+      <c r="E16" s="6">
+        <v>4.82E-2</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>